<commit_message>
Made edits to file
</commit_message>
<xml_diff>
--- a/FunctionCSV/SmoothedLogFunction.xlsx
+++ b/FunctionCSV/SmoothedLogFunction.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rache\IdeaProjects\Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rache\IdeaProjects\Project2\FunctionCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{59FDFB6C-ACC6-4C3B-802B-C7911CAF45EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C0C305-312E-4107-B087-A5B3F4E38E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{1DEDE39D-AC8E-48FA-8FFA-9E0FA906F5F7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="2" activeTab="3" xr2:uid="{1DEDE39D-AC8E-48FA-8FFA-9E0FA906F5F7}"/>
   </bookViews>
   <sheets>
     <sheet name="SmoothedLogFunctionWV250" sheetId="1" r:id="rId1"/>
@@ -28351,8 +28351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9E9AF3-DF75-46E8-8E4B-B9958FEAD4FF}">
   <dimension ref="A1:D1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -36379,7 +36379,7 @@
   <dimension ref="A1:D1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -44406,7 +44406,7 @@
   <dimension ref="A1:D1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -52432,8 +52432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA88ABE0-42A8-473A-A9DB-FC1B5749807A}">
   <dimension ref="A1:D1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>